<commit_message>
Corrections in the guidance
</commit_message>
<xml_diff>
--- a/How to translate Scratch Cards/Sizes.xlsx
+++ b/How to translate Scratch Cards/Sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\Scratch-Cards-Temp\Translating Scratch Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\Scratch-Cards-Temp\How to translate Scratch Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52BEF1-B1AD-421A-A88C-54A462486175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4562C43B-0686-400E-BA7C-F96C12941DCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4DFB14EF-77C2-4B96-A11E-35DC8632736A}"/>
+    <workbookView xWindow="1515" yWindow="2400" windowWidth="21600" windowHeight="11835" xr2:uid="{4DFB14EF-77C2-4B96-A11E-35DC8632736A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -414,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0698B882-AFF6-46F3-BD85-FB3E9E0C8D13}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,6 +558,40 @@
         <v>1.1851851851851851</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>106</v>
+      </c>
+      <c r="C20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>805</v>
+      </c>
+      <c r="C21">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f>SUM(B19:B21)</f>
+        <v>914</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C19:C21)</f>
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>